<commit_message>
Added start and end times to general comments
</commit_message>
<xml_diff>
--- a/Data_irregularities/Data_irregularities.xlsx
+++ b/Data_irregularities/Data_irregularities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmitta\DataDescriptor\Production-Data-Set-for-Five-Axis-CNC-Milling-with-Multiple-Changeovers\Data_irregularities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ECD521-99B1-4A58-AC94-DA2B9A76CB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4DADAD-47F1-437D-B6E7-E63BD2C37A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51F1E3C-909D-0548-B424-4B43210C78C2}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="German" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">English!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">German!$A$1:$I$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="129">
   <si>
     <t>Phase</t>
   </si>
@@ -170,12 +171,6 @@
     <t>Verzögerung beim Einlagern der Werkzeug</t>
   </si>
   <si>
-    <t>Werkzeug welches gerüstet werden muss war bereits in der Anlage - Keine Phase 41 in Rüstmatrix 3 vorhanden</t>
-  </si>
-  <si>
-    <t>Allgemein</t>
-  </si>
-  <si>
     <t>Hier Reinigungsaufwand kürzer als bei allen anderen - Verschmutzung war hier nicht so stark</t>
   </si>
   <si>
@@ -243,9 +238,6 @@
     <t>Einrichtteil defekt - falsche Maße eingetragen - Maschine musste erneut eingestellt werden</t>
   </si>
   <si>
-    <t>Ergänzung</t>
-  </si>
-  <si>
     <t>Haupttätigkeit Rüsten
 längere Phase</t>
   </si>
@@ -337,9 +329,6 @@
     <t>Delay wrong tool removed from storage - long</t>
   </si>
   <si>
-    <t>Delay bei Einlagerung Werkzeug - keine Notiz vorhanden - Wahrscheinlich Suche nach passender Einstellung für Bearbeitung</t>
-  </si>
-  <si>
     <t>Clamp blank product - door was not opened again but remained open!</t>
   </si>
   <si>
@@ -383,9 +372,6 @@
     <t>Delay when storing the tools</t>
   </si>
   <si>
-    <t>Tool that needs to be set up was already in the system - No phase 41 available in changeover matrix 3</t>
-  </si>
-  <si>
     <t>In general, many phases of changeover matrix 1 took significantly longer</t>
   </si>
   <si>
@@ -398,9 +384,6 @@
     <t>In contrast to all other recordings, all tools were swapped out the first time, even if they are actually needed for the next processing. In the other 4 recordings, only the tools that were not required for the next processing were removed.</t>
   </si>
   <si>
-    <t>Additionnal Comment</t>
-  </si>
-  <si>
     <t>Changeover</t>
   </si>
   <si>
@@ -416,10 +399,40 @@
     <t>42 to 45</t>
   </si>
   <si>
-    <t>General</t>
-  </si>
-  <si>
     <t>workpiece stopper had to be readjusted</t>
+  </si>
+  <si>
+    <t>Delay bei Einlagerung Werkzeug - Probably searching for suitable setting for machining</t>
+  </si>
+  <si>
+    <t>39 to 41</t>
+  </si>
+  <si>
+    <t>Tool that needs to be set up was already in the system - No phases 39 to 41 available in changeover matrix 3</t>
+  </si>
+  <si>
+    <t>Tool that needs to be set up was already in the system - No phases 42 to 45 available in changeover matrix 3</t>
+  </si>
+  <si>
+    <t>39 bis 41</t>
+  </si>
+  <si>
+    <t>Werkzeug welches gerüstet werden muss war bereits in der Anlage - Keine Phasen 42 bis 45 in Rüstmatrix 3 vorhanden</t>
+  </si>
+  <si>
+    <t>Werkzeug welches gerüstet werden muss war bereits in der Anlage - Keine Phasen 39 bis 41 in Rüstmatrix 3 vorhanden</t>
+  </si>
+  <si>
+    <t>1 bis 73</t>
+  </si>
+  <si>
+    <t>1 to 73</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Alle</t>
   </si>
 </sst>
 </file>
@@ -451,17 +464,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -541,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -565,7 +577,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,12 +584,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -589,6 +594,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,16 +946,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC09611-277E-498C-8707-88FC17C8C9B2}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="16"/>
-    <col min="3" max="3" width="18.21875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="13"/>
+    <col min="3" max="3" width="18.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="98.33203125" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
@@ -949,28 +965,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="40.5">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -984,13 +1000,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G2" s="8">
         <v>45363.362893518519</v>
@@ -1010,13 +1026,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G3" s="8">
         <v>45363.381157407406</v>
@@ -1036,13 +1052,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G4" s="8">
         <v>45363.399675925924</v>
@@ -1062,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G5" s="8">
         <v>45363.407002314816</v>
@@ -1088,13 +1104,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G6" s="8">
         <v>45363.422673611109</v>
@@ -1114,13 +1130,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G7" s="8">
         <v>45363.439097222225</v>
@@ -1140,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G8" s="8">
         <v>45363.448657407411</v>
@@ -1166,13 +1182,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G9" s="8">
         <v>45363.450810185182</v>
@@ -1192,13 +1208,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="G10" s="8">
         <v>45363.453356481485</v>
@@ -1218,13 +1234,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="G11" s="8">
         <v>45363.458171296297</v>
@@ -1244,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G12" s="8">
         <v>45363.459178240744</v>
@@ -1270,13 +1286,13 @@
         <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G13" s="8">
         <v>45363.549421296295</v>
@@ -1296,13 +1312,13 @@
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G14" s="8">
         <v>45363.552743055552</v>
@@ -1322,13 +1338,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G15" s="8">
         <v>45363.570104166669</v>
@@ -1348,13 +1364,13 @@
         <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G16" s="8">
         <v>45371.283043981479</v>
@@ -1363,7 +1379,7 @@
         <v>45371.285173611112</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30">
+    <row r="17" spans="1:8">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1374,13 +1390,13 @@
         <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="G17" s="8">
         <v>45371.285821759258</v>
@@ -1400,13 +1416,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G18" s="8">
         <v>45371.300196759257</v>
@@ -1426,13 +1442,13 @@
         <v>2</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G19" s="8">
         <v>45371.329756944448</v>
@@ -1452,13 +1468,13 @@
         <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G20" s="8">
         <v>45371.347210648149</v>
@@ -1478,13 +1494,13 @@
         <v>2</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G21" s="8">
         <v>45371.350659722222</v>
@@ -1503,14 +1519,14 @@
       <c r="C22" s="6">
         <v>2</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>93</v>
+      <c r="D22" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G22" s="8">
         <v>45371.390416666669</v>
@@ -1530,13 +1546,13 @@
         <v>3</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G23" s="8">
         <v>45371.442835648151</v>
@@ -1556,13 +1572,13 @@
         <v>3</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G24" s="8">
         <v>45371.456932870373</v>
@@ -1582,13 +1598,13 @@
         <v>3</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G25" s="8">
         <v>45371.459988425922</v>
@@ -1604,17 +1620,17 @@
       <c r="B26" s="6">
         <v>41</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <v>4</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>120</v>
+      <c r="D26" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G26" s="8">
         <v>45373.324444444443</v>
@@ -1634,13 +1650,13 @@
         <v>4</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G27" s="8">
         <v>45373.352627314816</v>
@@ -1660,13 +1676,13 @@
         <v>5</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G28" s="8">
         <v>45373.367743055554</v>
@@ -1686,13 +1702,13 @@
         <v>5</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>120</v>
+        <v>71</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G29" s="8">
         <v>45373.409085648149</v>
@@ -1712,13 +1728,13 @@
         <v>5</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G30" s="8">
         <v>45373.431284722225</v>
@@ -1738,13 +1754,13 @@
         <v>5</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G31" s="8">
         <v>45373.451261574075</v>
@@ -1764,13 +1780,13 @@
         <v>5</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G32" s="8">
         <v>45373.451736111114</v>
@@ -1790,13 +1806,13 @@
         <v>5</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G33" s="8">
         <v>45373.473993055559</v>
@@ -1805,8 +1821,8 @@
         <v>45373.474606481483</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75">
-      <c r="A34" s="12">
+    <row r="34" spans="1:8">
+      <c r="A34" s="17">
         <v>33</v>
       </c>
       <c r="B34" s="6">
@@ -1816,22 +1832,22 @@
         <v>1</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>120</v>
+        <v>90</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="45.75">
+        <v>105</v>
+      </c>
+      <c r="G34" s="8">
+        <v>45363.575613425928</v>
+      </c>
+      <c r="H34" s="8">
+        <v>45363.576284722221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="45">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -1842,22 +1858,22 @@
         <v>2</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75">
+        <v>106</v>
+      </c>
+      <c r="G35" s="15">
+        <v>45371.390810185185</v>
+      </c>
+      <c r="H35" s="15">
+        <v>45371.392280092594</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -1868,22 +1884,22 @@
         <v>1</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75">
+        <v>107</v>
+      </c>
+      <c r="G36" s="15">
+        <v>45363.349340277775</v>
+      </c>
+      <c r="H36" s="15">
+        <v>45363.35015046296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -1894,100 +1910,100 @@
         <v>1</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>120</v>
+        <v>92</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="45.75">
+        <v>105</v>
+      </c>
+      <c r="G37" s="15">
+        <v>45363.354872685188</v>
+      </c>
+      <c r="H37" s="15">
+        <v>45363.35628472222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="45">
       <c r="A38" s="6">
         <v>37</v>
       </c>
-      <c r="B38" s="6">
-        <v>41</v>
+      <c r="B38" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="C38" s="6">
         <v>3</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75">
+        <v>120</v>
+      </c>
+      <c r="G38" s="15">
+        <v>45371.398865740739</v>
+      </c>
+      <c r="H38" s="15">
+        <v>45371.398877314816</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="6">
         <v>38</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>123</v>
+      <c r="B39" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="C39" s="6">
         <v>1</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>120</v>
+        <v>127</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75">
+        <v>108</v>
+      </c>
+      <c r="G39" s="15">
+        <v>45363.344502314816</v>
+      </c>
+      <c r="H39" s="15">
+        <v>45363.577199074076</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="6">
         <v>39</v>
       </c>
-      <c r="B40" s="15">
-        <v>12</v>
+      <c r="B40" s="12">
+        <v>3</v>
       </c>
       <c r="C40" s="6">
         <v>4</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>120</v>
+        <v>81</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75">
+        <v>109</v>
+      </c>
+      <c r="G40" s="15">
+        <v>45371.586273148147</v>
+      </c>
+      <c r="H40" s="15">
+        <v>45371.586712962962</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -1998,74 +2014,75 @@
         <v>1</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>120</v>
+        <v>88</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="45.75">
+        <v>110</v>
+      </c>
+      <c r="G41" s="15">
+        <v>45363.52784722222</v>
+      </c>
+      <c r="H41" s="15">
+        <v>45363.528402777774</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="45">
       <c r="A42" s="6">
         <v>41</v>
       </c>
-      <c r="B42" s="15" t="s">
-        <v>121</v>
+      <c r="B42" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="C42" s="6">
         <v>1</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="45.75">
+        <v>111</v>
+      </c>
+      <c r="G42" s="15">
+        <v>45363.529907407406</v>
+      </c>
+      <c r="H42" s="15">
+        <v>45363.530393518522</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="45">
       <c r="A43" s="6">
         <v>42</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>122</v>
+      <c r="B43" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="C43" s="6">
         <v>3</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>117</v>
+        <v>121</v>
+      </c>
+      <c r="G43" s="16">
+        <v>45371.410983796297</v>
+      </c>
+      <c r="H43" s="16">
+        <v>45371.410995370374</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{0DC09611-277E-498C-8707-88FC17C8C9B2}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2075,15 +2092,16 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView zoomScale="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="18"/>
+    <col min="3" max="3" width="18.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="98.33203125" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
@@ -2093,7 +2111,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40.5">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2117,7 +2135,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30">
@@ -2134,7 +2152,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>7</v>
@@ -2146,7 +2164,7 @@
         <v>45363.362893518519</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30">
@@ -2175,7 +2193,7 @@
         <v>45363.399664351855</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30">
@@ -2204,7 +2222,7 @@
         <v>45363.405543981484</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30">
@@ -2233,7 +2251,7 @@
         <v>45363.40896990741</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2262,7 +2280,7 @@
         <v>45363.424074074072</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30">
@@ -2291,7 +2309,7 @@
         <v>45363.440115740741</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30">
@@ -2308,7 +2326,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>18</v>
@@ -2320,7 +2338,7 @@
         <v>45363.450601851851</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
@@ -2349,7 +2367,7 @@
         <v>45363.451215277775</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30">
@@ -2378,7 +2396,7 @@
         <v>45363.453750000001</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30">
@@ -2407,7 +2425,7 @@
         <v>45363.458275462966</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2436,7 +2454,7 @@
         <v>45363.459768518522</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2465,7 +2483,7 @@
         <v>45363.552152777775</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30">
@@ -2494,7 +2512,7 @@
         <v>45363.554074074076</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30">
@@ -2511,7 +2529,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>26</v>
@@ -2523,7 +2541,7 @@
         <v>45363.570243055554</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2543,7 +2561,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G16" s="8">
         <v>45371.283043981479</v>
@@ -2552,7 +2570,7 @@
         <v>45371.285173611112</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
@@ -2572,7 +2590,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G17" s="8">
         <v>45371.285821759258</v>
@@ -2581,7 +2599,7 @@
         <v>45371.286620370367</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45">
@@ -2598,7 +2616,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>28</v>
@@ -2610,7 +2628,7 @@
         <v>45371.300613425927</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30">
@@ -2627,7 +2645,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>29</v>
@@ -2639,7 +2657,7 @@
         <v>45371.331377314818</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30">
@@ -2656,7 +2674,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>37</v>
@@ -2668,7 +2686,7 @@
         <v>45371.348946759259</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30">
@@ -2688,7 +2706,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G21" s="8">
         <v>45371.350659722222</v>
@@ -2697,7 +2715,7 @@
         <v>45371.351400462961</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45">
@@ -2710,11 +2728,11 @@
       <c r="C22" s="6">
         <v>2</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>30</v>
@@ -2726,7 +2744,7 @@
         <v>45371.390787037039</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30">
@@ -2743,7 +2761,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>31</v>
@@ -2755,7 +2773,7 @@
         <v>45371.444421296299</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30">
@@ -2772,7 +2790,7 @@
         <v>17</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>32</v>
@@ -2784,7 +2802,7 @@
         <v>45371.457199074073</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30">
@@ -2813,7 +2831,7 @@
         <v>45371.460347222222</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="60">
@@ -2823,17 +2841,17 @@
       <c r="B26" s="6">
         <v>41</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <v>4</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>58</v>
+      <c r="E26" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G26" s="8">
         <v>45373.324444444443</v>
@@ -2842,7 +2860,7 @@
         <v>45373.324699074074</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2871,7 +2889,7 @@
         <v>45373.35633101852</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2891,7 +2909,7 @@
         <v>13</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G28" s="8">
         <v>45373.367743055554</v>
@@ -2900,7 +2918,7 @@
         <v>45373.368981481479</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2929,7 +2947,7 @@
         <v>45373.41202546296</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30">
@@ -2958,7 +2976,7 @@
         <v>45373.432071759256</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30">
@@ -2987,7 +3005,7 @@
         <v>45373.451458333337</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30">
@@ -3016,7 +3034,7 @@
         <v>45373.452800925923</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30">
@@ -3045,20 +3063,20 @@
         <v>45373.474606481483</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="30.75">
-      <c r="A34" s="12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30">
+      <c r="A34" s="17">
         <v>33</v>
       </c>
       <c r="B34" s="6">
         <v>59</v>
       </c>
-      <c r="C34" s="9">
-        <v>1</v>
-      </c>
-      <c r="D34" s="9" t="s">
+      <c r="C34" s="12">
+        <v>1</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="7" t="s">
@@ -3067,85 +3085,85 @@
       <c r="F34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>66</v>
+      <c r="G34" s="8">
+        <v>45363.575613425928</v>
+      </c>
+      <c r="H34" s="8">
+        <v>45363.576284722221</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="45.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="45">
       <c r="A35" s="6">
         <v>34</v>
       </c>
       <c r="B35" s="6">
         <v>49</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="12">
         <v>2</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30.75">
+      <c r="G35" s="15">
+        <v>45371.390810185185</v>
+      </c>
+      <c r="H35" s="15">
+        <v>45371.392280092594</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30">
       <c r="A36" s="6">
         <v>35</v>
       </c>
       <c r="B36" s="6">
         <v>41</v>
       </c>
-      <c r="C36" s="9">
-        <v>1</v>
-      </c>
-      <c r="D36" s="9" t="s">
+      <c r="C36" s="12">
+        <v>1</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G36" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>66</v>
+      <c r="G36" s="15">
+        <v>45363.349340277775</v>
+      </c>
+      <c r="H36" s="15">
+        <v>45363.35015046296</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30">
       <c r="A37" s="6">
         <v>36</v>
       </c>
       <c r="B37" s="6">
         <v>59</v>
       </c>
-      <c r="C37" s="9">
-        <v>1</v>
-      </c>
-      <c r="D37" s="9" t="s">
+      <c r="C37" s="12">
+        <v>1</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -3154,188 +3172,188 @@
       <c r="F37" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>66</v>
+      <c r="G37" s="15">
+        <v>45363.354872685188</v>
+      </c>
+      <c r="H37" s="15">
+        <v>45363.35628472222</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="45.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="45">
       <c r="A38" s="6">
         <v>37</v>
       </c>
-      <c r="B38" s="6">
-        <v>41</v>
-      </c>
-      <c r="C38" s="9">
+      <c r="B38" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="12">
         <v>3</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="30.75">
+        <v>124</v>
+      </c>
+      <c r="G38" s="15">
+        <v>45371.398865740739</v>
+      </c>
+      <c r="H38" s="15">
+        <v>45371.398877314816</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30">
       <c r="A39" s="6">
         <v>38</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="9">
-        <v>1</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>15</v>
+      <c r="B39" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="G39" s="15">
+        <v>45363.344502314816</v>
+      </c>
+      <c r="H39" s="15">
+        <v>45363.577199074076</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="30.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30">
       <c r="A40" s="6">
         <v>39</v>
       </c>
       <c r="B40" s="6">
-        <v>12</v>
-      </c>
-      <c r="C40" s="9">
+        <v>3</v>
+      </c>
+      <c r="C40" s="12">
         <v>4</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="12" t="s">
         <v>15</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>66</v>
+        <v>42</v>
+      </c>
+      <c r="G40" s="15">
+        <v>45371.586273148147</v>
+      </c>
+      <c r="H40" s="15">
+        <v>45371.586712962962</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="30.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30">
       <c r="A41" s="6">
         <v>40</v>
       </c>
       <c r="B41" s="6">
         <v>4</v>
       </c>
-      <c r="C41" s="9">
-        <v>1</v>
-      </c>
-      <c r="D41" s="9" t="s">
+      <c r="C41" s="12">
+        <v>1</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>66</v>
+        <v>43</v>
+      </c>
+      <c r="G41" s="15">
+        <v>45363.52784722222</v>
+      </c>
+      <c r="H41" s="15">
+        <v>45363.528402777774</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="45.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="45">
       <c r="A42" s="6">
         <v>41</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="9">
-        <v>1</v>
-      </c>
-      <c r="D42" s="9" t="s">
+      <c r="B42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="12">
+        <v>1</v>
+      </c>
+      <c r="D42" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="45.75">
+        <v>45</v>
+      </c>
+      <c r="G42" s="15">
+        <v>45363.529907407406</v>
+      </c>
+      <c r="H42" s="15">
+        <v>45363.530393518522</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45">
       <c r="A43" s="6">
         <v>42</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="9">
+      <c r="B43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="12">
         <v>3</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>63</v>
+        <v>123</v>
+      </c>
+      <c r="G43" s="16">
+        <v>45371.410983796297</v>
+      </c>
+      <c r="H43" s="16">
+        <v>45371.410995370374</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>